<commit_message>
all working and writing image files for each processing stage(120 in total)
</commit_message>
<xml_diff>
--- a/feature_sorting/fs_results.xlsx
+++ b/feature_sorting/fs_results.xlsx
@@ -432,28 +432,28 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1950</v>
+        <v>1.827676240208877</v>
       </c>
       <c r="C2">
-        <v>1764</v>
+        <v>0.3952569169960474</v>
       </c>
       <c r="D2">
-        <v>1919</v>
+        <v>5.839057899901865</v>
       </c>
       <c r="E2">
-        <v>1611</v>
+        <v>1.648351648351648</v>
       </c>
       <c r="F2">
-        <v>1813</v>
+        <v>0.6575342465753425</v>
       </c>
       <c r="G2">
-        <v>1456</v>
+        <v>0.06863417982155114</v>
       </c>
       <c r="H2">
-        <v>1956</v>
+        <v>0.1531393568147014</v>
       </c>
       <c r="I2">
-        <v>1897</v>
+        <v>0.1055408970976253</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -461,28 +461,28 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1939</v>
+        <v>1.253263707571802</v>
       </c>
       <c r="C3">
-        <v>1764</v>
+        <v>0.7315700619020821</v>
       </c>
       <c r="D3">
-        <v>1918</v>
+        <v>6.026457618814306</v>
       </c>
       <c r="E3">
-        <v>1609</v>
+        <v>2.188449848024316</v>
       </c>
       <c r="F3">
-        <v>1823</v>
+        <v>0.1098297638660077</v>
       </c>
       <c r="G3">
-        <v>1450</v>
+        <v>0.7529089664613279</v>
       </c>
       <c r="H3">
-        <v>1957</v>
+        <v>0.05107252298263534</v>
       </c>
       <c r="I3">
-        <v>1900</v>
+        <v>0.2109704641350211</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -490,28 +490,28 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1826</v>
+        <v>4.647519582245431</v>
       </c>
       <c r="C4">
-        <v>1867</v>
+        <v>5.420666290231508</v>
       </c>
       <c r="D4">
-        <v>1916</v>
+        <v>6.032368808239333</v>
       </c>
       <c r="E4">
-        <v>1605</v>
+        <v>2.134146341463415</v>
       </c>
       <c r="F4">
-        <v>1813</v>
+        <v>0.4939626783754116</v>
       </c>
       <c r="G4">
-        <v>1452</v>
+        <v>0.3431708991077557</v>
       </c>
       <c r="H4">
-        <v>1955</v>
+        <v>0.0511770726714432</v>
       </c>
       <c r="I4">
-        <v>1812</v>
+        <v>4.931794333683106</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -519,28 +519,28 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2199</v>
+        <v>14.83028720626632</v>
       </c>
       <c r="C5">
-        <v>2311</v>
+        <v>30.63877897117015</v>
       </c>
       <c r="D5">
-        <v>1919</v>
+        <v>5.977462028417443</v>
       </c>
       <c r="E5">
-        <v>1610</v>
+        <v>1.769371568029286</v>
       </c>
       <c r="F5">
-        <v>1813</v>
+        <v>0.4393190554640308</v>
       </c>
       <c r="G5">
-        <v>1486</v>
+        <v>2.200825309491059</v>
       </c>
       <c r="H5">
-        <v>1953</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1898</v>
+        <v>0.0526592943654555</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -548,28 +548,28 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1935</v>
+        <v>0.8337675872850442</v>
       </c>
       <c r="C6">
-        <v>1765</v>
+        <v>0.4512126339537508</v>
       </c>
       <c r="D6">
-        <v>1921</v>
+        <v>5.740922473012758</v>
       </c>
       <c r="E6">
-        <v>1611</v>
+        <v>1.828153564899452</v>
       </c>
       <c r="F6">
-        <v>1829</v>
+        <v>0.3841931942919868</v>
       </c>
       <c r="G6">
-        <v>1488</v>
+        <v>1.987662782727896</v>
       </c>
       <c r="H6">
-        <v>1956</v>
+        <v>0.2549719530851606</v>
       </c>
       <c r="I6">
-        <v>1794</v>
+        <v>5.628616517622304</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -577,28 +577,28 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1921</v>
+        <v>0.5232862375719518</v>
       </c>
       <c r="C7">
-        <v>1765</v>
+        <v>0.2261164499717354</v>
       </c>
       <c r="D7">
-        <v>1912</v>
+        <v>6.136475208640157</v>
       </c>
       <c r="E7">
-        <v>1609</v>
+        <v>1.830384380719951</v>
       </c>
       <c r="F7">
-        <v>1820</v>
+        <v>0.1097694840834248</v>
       </c>
       <c r="G7">
-        <v>1495</v>
+        <v>2.537722908093278</v>
       </c>
       <c r="H7">
-        <v>1852</v>
+        <v>5.413687436159346</v>
       </c>
       <c r="I7">
-        <v>1741</v>
+        <v>8.175105485232068</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -606,28 +606,28 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2076</v>
+        <v>8.407310704960835</v>
       </c>
       <c r="C8">
-        <v>1423</v>
+        <v>19.37677053824363</v>
       </c>
       <c r="D8">
-        <v>1909</v>
+        <v>6.237721021611002</v>
       </c>
       <c r="E8">
-        <v>1609</v>
+        <v>1.830384380719951</v>
       </c>
       <c r="F8">
-        <v>1819</v>
+        <v>0.1646542261251372</v>
       </c>
       <c r="G8">
-        <v>1496</v>
+        <v>2.747252747252747</v>
       </c>
       <c r="H8">
-        <v>1852</v>
+        <v>5.316973415132924</v>
       </c>
       <c r="I8">
-        <v>1744</v>
+        <v>8.258811152025251</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -635,28 +635,28 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1927</v>
+        <v>0.6266318537859008</v>
       </c>
       <c r="C9">
-        <v>1768</v>
+        <v>0.1693958215697346</v>
       </c>
       <c r="D9">
-        <v>1911</v>
+        <v>6.185567010309279</v>
       </c>
       <c r="E9">
-        <v>1613</v>
+        <v>1.825928180158247</v>
       </c>
       <c r="F9">
-        <v>1834</v>
+        <v>0.7138934651290499</v>
       </c>
       <c r="G9">
-        <v>1449</v>
+        <v>0.6172839506172839</v>
       </c>
       <c r="H9">
-        <v>1956</v>
+        <v>0.3058103975535168</v>
       </c>
       <c r="I9">
-        <v>1899</v>
+        <v>0.2110817941952506</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -664,28 +664,28 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1914</v>
+        <v>0.05227391531625718</v>
       </c>
       <c r="C10">
-        <v>1444</v>
+        <v>18.32579185520362</v>
       </c>
       <c r="D10">
-        <v>1917</v>
+        <v>5.937193326790972</v>
       </c>
       <c r="E10">
-        <v>1611</v>
+        <v>1.94765672550213</v>
       </c>
       <c r="F10">
-        <v>1832</v>
+        <v>0.6040637012630422</v>
       </c>
       <c r="G10">
-        <v>1463</v>
+        <v>0.2741603838245374</v>
       </c>
       <c r="H10">
-        <v>1850</v>
+        <v>5.660377358490567</v>
       </c>
       <c r="I10">
-        <v>1746</v>
+        <v>7.61904761904762</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -693,28 +693,28 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1923</v>
+        <v>0.5227391531625719</v>
       </c>
       <c r="C11">
-        <v>1761</v>
+        <v>0.226628895184136</v>
       </c>
       <c r="D11">
-        <v>1918</v>
+        <v>5.795677799607073</v>
       </c>
       <c r="E11">
-        <v>1611</v>
+        <v>1.887941534713764</v>
       </c>
       <c r="F11">
-        <v>1815</v>
+        <v>0.2747252747252747</v>
       </c>
       <c r="G11">
-        <v>1472</v>
+        <v>1.517241379310345</v>
       </c>
       <c r="H11">
-        <v>1852</v>
+        <v>5.750636132315521</v>
       </c>
       <c r="I11">
-        <v>1744</v>
+        <v>7.871104067617539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>